<commit_message>
Update spreadsheet with new parameters from Maite
</commit_message>
<xml_diff>
--- a/selected_patients.xlsx
+++ b/selected_patients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - UPV\POSTDOC\Proyectos\SimCardioTest\Simula\7-ecg\Sent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/mamofe_upv_edu_es/Documents/POSTDOC/Proyectos/SimCardioTest/Simula/7-ecg/Sent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_AD4D2F04E46CFB4ACB3E20B34D14C904693EDF26" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4F6696F8-47F0-47EA-B104-1D4CBDD92970}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_AD4D2F04E46CFB4ACB3E20B34D14C904693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48E9386D-2A77-4330-847D-17F8AA8BB266}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -306,7 +317,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -475,42 +486,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,15 +801,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AA19"/>
+  <dimension ref="B3:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
         <v>1</v>
@@ -813,17 +823,17 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -832,14 +842,14 @@
       <c r="I4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -849,10 +859,10 @@
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="11">
-        <v>1</v>
-      </c>
-      <c r="F5" s="14">
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
         <f>C5*D5*E5</f>
         <v>1.4378</v>
       </c>
@@ -862,28 +872,15 @@
       <c r="I5" s="5">
         <v>1</v>
       </c>
-      <c r="J5" s="11">
-        <v>1</v>
-      </c>
-      <c r="K5" s="14">
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13">
         <f>H5*I5*J5</f>
         <v>1.1395</v>
       </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-    </row>
-    <row r="6" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -893,10 +890,10 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>2.274</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <f t="shared" ref="F6:F17" si="0">C6*D6*E6</f>
         <v>3.2695571999999999</v>
       </c>
@@ -907,10 +904,10 @@
       <c r="I6" s="4">
         <v>1</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="11">
         <v>2.274</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <f t="shared" ref="K6:K17" si="1">H6*I6*J6</f>
         <v>2.5912229999999998</v>
       </c>
@@ -926,9 +923,8 @@
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
-      <c r="AA6" s="9"/>
-    </row>
-    <row r="7" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -938,10 +934,10 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="11">
-        <v>1</v>
-      </c>
-      <c r="F7" s="14">
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>1.3478000000000001</v>
       </c>
@@ -951,15 +947,15 @@
       <c r="I7" s="5">
         <v>1</v>
       </c>
-      <c r="J7" s="11">
-        <v>1</v>
-      </c>
-      <c r="K7" s="14">
+      <c r="J7" s="10">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13">
         <f t="shared" si="1"/>
         <v>0.84989999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -967,14 +963,14 @@
         <v>0.84619999999999995</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11">
-        <v>1</v>
-      </c>
-      <c r="F8" s="14">
+        <v>0.82</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1.018</v>
+      </c>
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
-        <v>0.84619999999999995</v>
+        <v>0.70637391199999999</v>
       </c>
       <c r="H8" s="4">
         <v>1.5798000000000001</v>
@@ -982,19 +978,19 @@
       <c r="I8" s="5">
         <v>1</v>
       </c>
-      <c r="J8" s="11">
-        <v>1</v>
-      </c>
-      <c r="K8" s="14">
+      <c r="J8" s="10">
+        <v>1.018</v>
+      </c>
+      <c r="K8" s="13">
         <f t="shared" si="1"/>
-        <v>1.5798000000000001</v>
+        <v>1.6082364</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1004,10 +1000,10 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>1.119</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <f t="shared" si="0"/>
         <v>0.96659220000000001</v>
       </c>
@@ -1017,16 +1013,16 @@
       <c r="I9" s="5">
         <v>0.98</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>1.119</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <f t="shared" si="1"/>
         <v>1.0196372759999999</v>
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1036,10 +1032,10 @@
       <c r="D10" s="5">
         <v>1.4</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>1.6479999999999999</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <f t="shared" si="0"/>
         <v>2.4405561599999999</v>
       </c>
@@ -1049,16 +1045,16 @@
       <c r="I10" s="5">
         <v>1.19</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <v>1.6479999999999999</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <f t="shared" si="1"/>
         <v>1.5512459199999999</v>
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1068,10 +1064,10 @@
       <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>1.4139999999999999</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <f t="shared" si="0"/>
         <v>1.5027991999999999</v>
       </c>
@@ -1081,16 +1077,16 @@
       <c r="I11" s="5">
         <v>1</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>1.4139999999999999</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <f t="shared" si="1"/>
         <v>0.75889379999999984</v>
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1100,10 +1096,10 @@
       <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="11">
-        <v>1</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
         <f t="shared" si="0"/>
         <v>1.0253000000000001</v>
       </c>
@@ -1113,16 +1109,16 @@
       <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="J12" s="11">
-        <v>1</v>
-      </c>
-      <c r="K12" s="14">
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
+      <c r="K12" s="13">
         <f t="shared" si="1"/>
         <v>0.81279999999999997</v>
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1132,10 +1128,10 @@
       <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="11">
-        <v>1</v>
-      </c>
-      <c r="F13" s="14">
+      <c r="E13" s="10">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13">
         <f t="shared" si="0"/>
         <v>0.30180000000000001</v>
       </c>
@@ -1145,16 +1141,16 @@
       <c r="I13" s="5">
         <v>1</v>
       </c>
-      <c r="J13" s="11">
-        <v>1</v>
-      </c>
-      <c r="K13" s="14">
+      <c r="J13" s="10">
+        <v>1</v>
+      </c>
+      <c r="K13" s="13">
         <f t="shared" si="1"/>
         <v>0.29580000000000001</v>
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1164,10 +1160,10 @@
       <c r="D14" s="5">
         <v>1</v>
       </c>
-      <c r="E14" s="11">
-        <v>1</v>
-      </c>
-      <c r="F14" s="14">
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
         <f t="shared" si="0"/>
         <v>0.79979999999999996</v>
       </c>
@@ -1177,16 +1173,16 @@
       <c r="I14" s="5">
         <v>1</v>
       </c>
-      <c r="J14" s="11">
-        <v>1</v>
-      </c>
-      <c r="K14" s="14">
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13">
         <f t="shared" si="1"/>
         <v>1.7695000000000001</v>
       </c>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1194,14 +1190,14 @@
         <v>0.97060000000000002</v>
       </c>
       <c r="D15" s="5">
-        <v>0.82</v>
-      </c>
-      <c r="E15" s="11">
-        <v>1.018</v>
-      </c>
-      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
         <f t="shared" si="0"/>
-        <v>0.81021805599999996</v>
+        <v>0.97060000000000002</v>
       </c>
       <c r="H15" s="4">
         <v>1.0026999999999999</v>
@@ -1209,16 +1205,16 @@
       <c r="I15" s="5">
         <v>1</v>
       </c>
-      <c r="J15" s="11">
-        <v>1.018</v>
-      </c>
-      <c r="K15" s="14">
+      <c r="J15" s="10">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13">
         <f t="shared" si="1"/>
-        <v>1.0207485999999999</v>
+        <v>1.0026999999999999</v>
       </c>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="2:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1228,10 +1224,10 @@
       <c r="D16" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="11">
-        <v>1</v>
-      </c>
-      <c r="F16" s="14">
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
         <f t="shared" si="0"/>
         <v>0.95940000000000003</v>
       </c>
@@ -1241,10 +1237,12 @@
       <c r="I16" s="5">
         <v>1</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="14">
+      <c r="J16" s="10">
+        <v>1</v>
+      </c>
+      <c r="K16" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.93830000000000002</v>
       </c>
       <c r="M16" s="8"/>
     </row>
@@ -1258,10 +1256,10 @@
       <c r="D17" s="5">
         <v>1</v>
       </c>
-      <c r="E17" s="11">
-        <v>1</v>
-      </c>
-      <c r="F17" s="16">
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
         <f t="shared" si="0"/>
         <v>1.0496000000000001</v>
       </c>
@@ -1271,10 +1269,10 @@
       <c r="I17" s="5">
         <v>1</v>
       </c>
-      <c r="J17" s="11">
-        <v>1</v>
-      </c>
-      <c r="K17" s="16">
+      <c r="J17" s="10">
+        <v>1</v>
+      </c>
+      <c r="K17" s="15">
         <f t="shared" si="1"/>
         <v>1.4383999999999999</v>
       </c>

</xml_diff>

<commit_message>
Add new scaling factors for profile2
</commit_message>
<xml_diff>
--- a/selected_patients.xlsx
+++ b/selected_patients.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/mamofe_upv_edu_es/Documents/POSTDOC/Proyectos/SimCardioTest/Simula/7-ecg/Sent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_AD4D2F04E46CFB4ACB3E20B34D14C904693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48E9386D-2A77-4330-847D-17F8AA8BB266}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="14_{3A0497F1-3722-449A-BFD8-05ACB8222689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B19D3940-FA4E-41A0-8E33-6049EE389AC9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="MedianCell" sheetId="2" r:id="rId1"/>
+    <sheet name="InitialSelection" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,6 +37,64 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mª Teresa Mora Fenoll</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{F1BF913F-2B30-49BC-BE7B-6D5A6D8D314A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mª Teresa Mora Fenoll:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Dihydrotestosterone 35 nM</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{4BA98F4E-B4E9-45AE-972E-4C2ED0EAE705}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mª Teresa Mora Fenoll:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+early follicular phase</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Mª Teresa Mora Fenoll</author>
@@ -94,12 +153,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>calm</t>
-  </si>
-  <si>
-    <t>MALE</t>
   </si>
   <si>
     <t>individual</t>
@@ -303,13 +359,28 @@
     <t>DHT</t>
   </si>
   <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
     <t>EFP</t>
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>PROFILE 1 (Llopis et al. 2023)</t>
+  </si>
+  <si>
+    <t>PROFILE 2 (Median APD in Mid cells)</t>
+  </si>
+  <si>
+    <t>MALE #50</t>
+  </si>
+  <si>
+    <t>FEMALE #74</t>
+  </si>
+  <si>
+    <t>MALE #6</t>
+  </si>
+  <si>
+    <t>FEMALE #35</t>
   </si>
 </sst>
 </file>
@@ -319,7 +390,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +444,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -486,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -521,6 +600,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,58 +880,556 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:Z19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C41DF8-E3E2-4C17-8643-338B8C23C160}">
+  <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="F4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.0705</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
+        <f>C5*D5*E5</f>
+        <v>1.0705</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.65910000000000002</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="13">
+        <f>H5*I5*J5</f>
+        <v>0.65910000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.0705</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
+        <v>2.274</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" ref="F6:F17" si="0">C6*D6*E6</f>
+        <v>2.4343170000000001</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4">
+        <v>0.65910000000000002</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2.274</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6:K17" si="1">H6*I6*J6</f>
+        <v>1.4987934000000001</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+    </row>
+    <row r="7" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.3165</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3165</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.93569999999999998</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13">
+        <f t="shared" si="1"/>
+        <v>0.93569999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.4489000000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1.018</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>1.209483764</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1.3217000000000001</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
+        <v>1.018</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" si="1"/>
+        <v>1.3454906000000002</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.9385</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1.119</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0501815000000001</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.98</v>
+      </c>
+      <c r="J9" s="10">
+        <v>1.119</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="1"/>
+        <v>0.72157596000000002</v>
+      </c>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1.6479999999999999</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>2.24952</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.80259999999999998</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1.19</v>
+      </c>
+      <c r="J10" s="10">
+        <v>1.6479999999999999</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" si="1"/>
+        <v>1.5739949119999996</v>
+      </c>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.67589999999999995</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
+        <v>0.95572259999999987</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.82650000000000001</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="1"/>
+        <v>1.168671</v>
+      </c>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.74690000000000001</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.74690000000000001</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.57920000000000005</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" si="1"/>
+        <v>0.57920000000000005</v>
+      </c>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.39829999999999999</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.39829999999999999</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.4249</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1</v>
+      </c>
+      <c r="K13" s="13">
+        <f t="shared" si="1"/>
+        <v>0.4249</v>
+      </c>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.2687999999999999</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
+        <v>1.2687999999999999</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1.3495999999999999</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" si="1"/>
+        <v>1.3495999999999999</v>
+      </c>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.6286</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>1.6286</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1.3057000000000001</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1</v>
+      </c>
+      <c r="K15" s="13">
+        <f t="shared" si="1"/>
+        <v>1.3057000000000001</v>
+      </c>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.5044999999999999</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="0"/>
+        <v>1.5044999999999999</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1.1108</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1</v>
+      </c>
+      <c r="J16" s="10">
+        <v>1</v>
+      </c>
+      <c r="K16" s="13">
+        <f t="shared" si="1"/>
+        <v>1.1108</v>
+      </c>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1.1102000000000001</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="0"/>
+        <v>1.1102000000000001</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1.2349000000000001</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1</v>
+      </c>
+      <c r="J17" s="10">
+        <v>1</v>
+      </c>
+      <c r="K17" s="15">
+        <f t="shared" si="1"/>
+        <v>1.2349000000000001</v>
+      </c>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="J4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="C5" s="4">
         <v>1.4378</v>
@@ -880,9 +1458,9 @@
         <v>1.1395</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4">
         <v>1.4378</v>
@@ -924,9 +1502,9 @@
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
     </row>
-    <row r="7" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4">
         <v>1.3478000000000001</v>
@@ -955,9 +1533,9 @@
         <v>0.84989999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4">
         <v>0.84619999999999995</v>
@@ -990,9 +1568,9 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4">
         <v>0.86380000000000001</v>
@@ -1022,9 +1600,9 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="4">
         <v>1.0578000000000001</v>
@@ -1054,9 +1632,9 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4">
         <v>1.0628</v>
@@ -1086,9 +1664,9 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
         <v>1.0253000000000001</v>
@@ -1118,9 +1696,9 @@
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
         <v>0.30180000000000001</v>
@@ -1150,9 +1728,9 @@
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4">
         <v>0.79979999999999996</v>
@@ -1182,9 +1760,9 @@
       </c>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4">
         <v>0.97060000000000002</v>
@@ -1214,9 +1792,9 @@
       </c>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="2:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="4">
         <v>0.95940000000000003</v>
@@ -1289,4 +1867,312 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fd20df89-4048-49a6-a67a-390eaa975cff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006E43017B494BB149B6A2335A5C790C9A" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fc1ac14bff2f537a589c06d2b3095714">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fd20df89-4048-49a6-a67a-390eaa975cff" xmlns:ns4="92ab9642-0aab-44de-b012-9f00b4c0dc56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="826b760cd4a02378e301654cfa6d95da" ns3:_="" ns4:_="">
+    <xsd:import namespace="fd20df89-4048-49a6-a67a-390eaa975cff"/>
+    <xsd:import namespace="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="fd20df89-4048-49a6-a67a-390eaa975cff" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="16" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="22" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="24" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="92ab9642-0aab-44de-b012-9f00b4c0dc56" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="20" nillable="true" ma:displayName="Hash de la sugerencia para compartir" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C4E15F1-20DF-4000-B95D-C70E4E10E749}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
+    <ds:schemaRef ds:uri="fd20df89-4048-49a6-a67a-390eaa975cff"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64639624-6B18-434B-A3B6-F52E5A89847D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8613E303-6A84-40F1-9DF0-E66925F3789D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fd20df89-4048-49a6-a67a-390eaa975cff"/>
+    <ds:schemaRef ds:uri="92ab9642-0aab-44de-b012-9f00b4c0dc56"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>